<commit_message>
create data 26.11.2015 jam 20.13
</commit_message>
<xml_diff>
--- a/files/btr.amr.112015.xlsx
+++ b/files/btr.amr.112015.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ECS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ECS\Documents\GitHub\3mm.3atur\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10230" windowHeight="6960"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="105">
   <si>
     <t>UNITUP</t>
   </si>
@@ -62,21 +62,30 @@
     <t>55200</t>
   </si>
   <si>
+    <t>552001180404</t>
+  </si>
+  <si>
+    <t>VILLA MESARI</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>JL SUWETA BENTUYUNG UBUD NO 0 UBUD GIANY</t>
+  </si>
+  <si>
     <t>552001023019</t>
   </si>
   <si>
     <t>LUH PUTRI DEWI SINTHAJANY</t>
   </si>
   <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>JL BISMA NO 0 UBUD KLOD</t>
   </si>
   <si>
@@ -89,15 +98,6 @@
     <t>JL RAYA BATUBULAN NO 0 TEGEHA</t>
   </si>
   <si>
-    <t>552001180404</t>
-  </si>
-  <si>
-    <t>VILLA MESARI</t>
-  </si>
-  <si>
-    <t>JL SUWETA BENTUYUNG UBUD NO 0 UBUD GIANY</t>
-  </si>
-  <si>
     <t>552000939702</t>
   </si>
   <si>
@@ -143,204 +143,168 @@
     <t>JL RY CELUK GG CELUK SESEH NO   SINGAPADU</t>
   </si>
   <si>
-    <t>552001099369</t>
-  </si>
-  <si>
-    <t>VILLA LOHIA</t>
-  </si>
-  <si>
-    <t>DN SAYAN UBUD DS BAUNG JAMBANGAN NO 0 UBUD</t>
-  </si>
-  <si>
-    <t>551200776655</t>
-  </si>
-  <si>
-    <t>ARTANA,ST I NYOMAN</t>
+    <t>552001207480</t>
+  </si>
+  <si>
+    <t>NI KETUT PURNITI</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>JL BATU INTAN SELATAN NO 0 BATUBULAN</t>
+  </si>
+  <si>
+    <t>551200766867</t>
+  </si>
+  <si>
+    <t>SILA I WAYAN</t>
+  </si>
+  <si>
+    <t>BR TENGKULAK KJ KAUH NO  KEMENUH</t>
+  </si>
+  <si>
+    <t>551200679026</t>
+  </si>
+  <si>
+    <t>SUWEDA I WAYAN</t>
+  </si>
+  <si>
+    <t>JL DS CANGGI NO 0 SAKAH</t>
+  </si>
+  <si>
+    <t>552001221522</t>
+  </si>
+  <si>
+    <t>ARIF SOELEMAN SIREGAR</t>
+  </si>
+  <si>
+    <t>DN PERANGSADA NO 0 PERING</t>
+  </si>
+  <si>
+    <t>551200422601</t>
+  </si>
+  <si>
+    <t>HOTEL ANOM SARI</t>
+  </si>
+  <si>
+    <t>JL LODTUNDUH NO 0 SILUNGAN</t>
+  </si>
+  <si>
+    <t>551200245212</t>
+  </si>
+  <si>
+    <t>PANTIASUHAN BALI GLOBAL A</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>BR BATAN ANCAK NO 0 MAS</t>
+  </si>
+  <si>
+    <t>551200462203</t>
+  </si>
+  <si>
+    <t>NI MADE MAWARNI</t>
+  </si>
+  <si>
+    <t>BR KAPAL NO 0 BATU BULAN</t>
+  </si>
+  <si>
+    <t>552001257523</t>
+  </si>
+  <si>
+    <t>I NENGAH NATYANTA</t>
+  </si>
+  <si>
+    <t>JL TEBONGKANG NO   SINGAKERTA</t>
+  </si>
+  <si>
+    <t>55230</t>
+  </si>
+  <si>
+    <t>552300508590</t>
+  </si>
+  <si>
+    <t>I GEDE ARKASENA WARDANA</t>
+  </si>
+  <si>
+    <t>DN BR DINAS LEBAH NO   SUKEDANA</t>
+  </si>
+  <si>
+    <t>552300361456</t>
+  </si>
+  <si>
+    <t>JUKIAN WAHYUDI</t>
+  </si>
+  <si>
+    <t>DN PEJENG NO 0 MENANGA</t>
+  </si>
+  <si>
+    <t>552300524096</t>
+  </si>
+  <si>
+    <t>I KOMANG WIRAWAN</t>
+  </si>
+  <si>
+    <t>DN MEKARSARI NO 0 SUKADANA</t>
+  </si>
+  <si>
+    <t>552300519758</t>
+  </si>
+  <si>
+    <t>I NYOMAN MURJANA</t>
+  </si>
+  <si>
+    <t>DS SELAT SEBUDI NO   SELAT</t>
+  </si>
+  <si>
+    <t>552300356778</t>
+  </si>
+  <si>
+    <t>RUSMAWATI</t>
+  </si>
+  <si>
+    <t>DN ANCUT NO 0 SEBUDI</t>
+  </si>
+  <si>
+    <t>552300594186</t>
+  </si>
+  <si>
+    <t>IR. A.A.K. SURYA TJANDRA</t>
+  </si>
+  <si>
+    <t>DS TUMBU, KARANGASEM NO - TUMBU</t>
+  </si>
+  <si>
+    <t>551570007672</t>
+  </si>
+  <si>
+    <t>EMERALD BEACH HOTEL</t>
+  </si>
+  <si>
+    <t>DN BATU DAWA KLOD NO 0 TULAMBEN</t>
+  </si>
+  <si>
+    <t>551550091397</t>
+  </si>
+  <si>
+    <t>PT MIAR HARVEST JAYA</t>
+  </si>
+  <si>
+    <t>BR YEH MALET NO 0 YEH MALET</t>
+  </si>
+  <si>
+    <t>552300565202</t>
+  </si>
+  <si>
+    <t>I GEDE BUDI HARTAWAN.ST</t>
   </si>
   <si>
     <t>R3</t>
   </si>
   <si>
-    <t>BR MAJANGAN NO  BUAHAN</t>
-  </si>
-  <si>
-    <t>552001207480</t>
-  </si>
-  <si>
-    <t>NI KETUT PURNITI</t>
-  </si>
-  <si>
-    <t>I2</t>
-  </si>
-  <si>
-    <t>JL BATU INTAN SELATAN NO 0 BATUBULAN</t>
-  </si>
-  <si>
-    <t>552001221522</t>
-  </si>
-  <si>
-    <t>ARIF SOELEMAN SIREGAR</t>
-  </si>
-  <si>
-    <t>DN PERANGSADA NO 0 PERING</t>
-  </si>
-  <si>
-    <t>551200245212</t>
-  </si>
-  <si>
-    <t>PANTIASUHAN BALI GLOBAL A</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>BR BATAN ANCAK NO 0 MAS</t>
-  </si>
-  <si>
-    <t>551200766867</t>
-  </si>
-  <si>
-    <t>SILA I WAYAN</t>
-  </si>
-  <si>
-    <t>BR TENGKULAK KJ KAUH NO  KEMENUH</t>
-  </si>
-  <si>
-    <t>551200422601</t>
-  </si>
-  <si>
-    <t>HOTEL ANOM SARI</t>
-  </si>
-  <si>
-    <t>JL LODTUNDUH NO 0 SILUNGAN</t>
-  </si>
-  <si>
-    <t>551200679026</t>
-  </si>
-  <si>
-    <t>SUWEDA I WAYAN</t>
-  </si>
-  <si>
-    <t>JL DS CANGGI NO 0 SAKAH</t>
-  </si>
-  <si>
-    <t>551230572182</t>
-  </si>
-  <si>
-    <t>DAVID S.KUNG</t>
-  </si>
-  <si>
-    <t>BR JUKUT PAKU NO 0 SINGAKERTA</t>
-  </si>
-  <si>
-    <t>552000979143</t>
-  </si>
-  <si>
-    <t>WIDODO</t>
-  </si>
-  <si>
-    <t>JL BY PASS I B MANTRA (SI0115/D1C4) NO 0 MANYAR</t>
-  </si>
-  <si>
-    <t>551200462203</t>
-  </si>
-  <si>
-    <t>NI MADE MAWARNI</t>
-  </si>
-  <si>
-    <t>BR KAPAL NO 0 BATU BULAN</t>
-  </si>
-  <si>
-    <t>552001257523</t>
-  </si>
-  <si>
-    <t>I NENGAH NATYANTA</t>
-  </si>
-  <si>
-    <t>JL TEBONGKANG NO   SINGAKERTA</t>
-  </si>
-  <si>
-    <t>55230</t>
-  </si>
-  <si>
-    <t>552300361456</t>
-  </si>
-  <si>
-    <t>JUKIAN WAHYUDI</t>
-  </si>
-  <si>
-    <t>DN PEJENG NO 0 MENANGA</t>
-  </si>
-  <si>
-    <t>552300508590</t>
-  </si>
-  <si>
-    <t>I GEDE ARKASENA WARDANA</t>
-  </si>
-  <si>
-    <t>DN BR DINAS LEBAH NO   SUKEDANA</t>
-  </si>
-  <si>
-    <t>552300524096</t>
-  </si>
-  <si>
-    <t>I KOMANG WIRAWAN</t>
-  </si>
-  <si>
-    <t>DN MEKARSARI NO 0 SUKADANA</t>
-  </si>
-  <si>
-    <t>552300519758</t>
-  </si>
-  <si>
-    <t>I NYOMAN MURJANA</t>
-  </si>
-  <si>
-    <t>DS SELAT SEBUDI NO   SELAT</t>
-  </si>
-  <si>
-    <t>552300356778</t>
-  </si>
-  <si>
-    <t>RUSMAWATI</t>
-  </si>
-  <si>
-    <t>DN ANCUT NO 0 SEBUDI</t>
-  </si>
-  <si>
-    <t>551570007672</t>
-  </si>
-  <si>
-    <t>EMERALD BEACH HOTEL</t>
-  </si>
-  <si>
-    <t>DN BATU DAWA KLOD NO 0 TULAMBEN</t>
-  </si>
-  <si>
-    <t>552300594186</t>
-  </si>
-  <si>
-    <t>IR. A.A.K. SURYA TJANDRA</t>
-  </si>
-  <si>
-    <t>DS TUMBU, KARANGASEM NO - TUMBU</t>
-  </si>
-  <si>
-    <t>551550091397</t>
-  </si>
-  <si>
-    <t>PT MIAR HARVEST JAYA</t>
-  </si>
-  <si>
-    <t>BR YEH MALET NO 0 YEH MALET</t>
-  </si>
-  <si>
-    <t>552300565202</t>
-  </si>
-  <si>
-    <t>I GEDE BUDI HARTAWAN.ST</t>
-  </si>
-  <si>
     <t>JL RAYA BUITAN NO 000 MANGGIS</t>
   </si>
   <si>
@@ -374,17 +338,15 @@
     <t>KL NUSA LEMBONGAN NO  JUNGUT BAT</t>
   </si>
   <si>
-    <t>No</t>
+    <t>NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -479,7 +441,7 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -490,7 +452,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="41" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -780,13 +741,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="72.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="69.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
@@ -795,15 +756,15 @@
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="67" customWidth="1"/>
     <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -832,10 +793,10 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -847,16 +808,16 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="3">
-        <v>197000</v>
+        <v>53000</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>15</v>
@@ -865,16 +826,16 @@
         <v>16</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="J2" s="3">
-        <v>1</v>
-      </c>
-      <c r="K2" s="6">
-        <v>16086260</v>
-      </c>
-      <c r="L2" s="6">
-        <v>438553</v>
+        <v>3</v>
+      </c>
+      <c r="K2" s="5">
+        <v>10342993</v>
+      </c>
+      <c r="L2" s="5">
+        <v>600000</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -885,16 +846,16 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="3">
-        <v>197000</v>
+        <v>147000</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>15</v>
@@ -903,16 +864,16 @@
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="J3" s="3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="6">
-        <v>12299911</v>
-      </c>
-      <c r="L3" s="6">
-        <v>335288</v>
+        <v>2</v>
+      </c>
+      <c r="K3" s="5">
+        <v>73773552</v>
+      </c>
+      <c r="L3" s="5">
+        <v>2986568</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -923,10 +884,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>14</v>
@@ -941,15 +902,15 @@
         <v>16</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J4" s="3">
         <v>1</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>13069109</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>356267</v>
       </c>
     </row>
@@ -961,16 +922,16 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="3">
-        <v>147000</v>
+        <v>197000</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>15</v>
@@ -979,16 +940,16 @@
         <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J5" s="3">
-        <v>2</v>
-      </c>
-      <c r="K5" s="6">
-        <v>73773552</v>
-      </c>
-      <c r="L5" s="6">
-        <v>2986568</v>
+        <v>1</v>
+      </c>
+      <c r="K5" s="5">
+        <v>16086260</v>
+      </c>
+      <c r="L5" s="5">
+        <v>438553</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -999,16 +960,16 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="3">
-        <v>105000</v>
+        <v>197000</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>15</v>
@@ -1017,16 +978,16 @@
         <v>16</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="J6" s="3">
         <v>1</v>
       </c>
-      <c r="K6" s="6">
-        <v>25402807</v>
-      </c>
-      <c r="L6" s="6">
-        <v>692640</v>
+      <c r="K6" s="5">
+        <v>12299911</v>
+      </c>
+      <c r="L6" s="5">
+        <v>335288</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1037,10 +998,10 @@
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>14</v>
@@ -1055,16 +1016,16 @@
         <v>16</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J7" s="3">
         <v>1</v>
       </c>
-      <c r="K7" s="6">
-        <v>6968571</v>
-      </c>
-      <c r="L7" s="6">
-        <v>189888</v>
+      <c r="K7" s="5">
+        <v>25402807</v>
+      </c>
+      <c r="L7" s="5">
+        <v>692640</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1075,10 +1036,10 @@
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>14</v>
@@ -1093,15 +1054,15 @@
         <v>16</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J8" s="3">
         <v>1</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>6968571</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="5">
         <v>189888</v>
       </c>
     </row>
@@ -1113,16 +1074,16 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="3">
-        <v>82500</v>
+        <v>105000</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>15</v>
@@ -1131,16 +1092,16 @@
         <v>16</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J9" s="3">
         <v>1</v>
       </c>
-      <c r="K9" s="6">
-        <v>5476592</v>
-      </c>
-      <c r="L9" s="6">
-        <v>149198</v>
+      <c r="K9" s="5">
+        <v>6968571</v>
+      </c>
+      <c r="L9" s="5">
+        <v>189888</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1151,10 +1112,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>14</v>
@@ -1169,16 +1130,16 @@
         <v>16</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J10" s="3">
-        <v>3</v>
-      </c>
-      <c r="K10" s="6">
-        <v>20713400</v>
-      </c>
-      <c r="L10" s="6">
-        <v>1048886</v>
+        <v>1</v>
+      </c>
+      <c r="K10" s="5">
+        <v>5476592</v>
+      </c>
+      <c r="L10" s="5">
+        <v>149198</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1189,13 +1150,13 @@
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F11" s="3">
         <v>66000</v>
@@ -1207,16 +1168,16 @@
         <v>16</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J11" s="3">
         <v>1</v>
       </c>
-      <c r="K11" s="6">
-        <v>9771684</v>
-      </c>
-      <c r="L11" s="6">
-        <v>244142</v>
+      <c r="K11" s="5">
+        <v>2649062</v>
+      </c>
+      <c r="L11" s="5">
+        <v>100000</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1227,16 +1188,16 @@
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F12" s="3">
-        <v>66000</v>
+        <v>53000</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>15</v>
@@ -1245,15 +1206,15 @@
         <v>16</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J12" s="3">
         <v>1</v>
       </c>
-      <c r="K12" s="6">
-        <v>2649062</v>
-      </c>
-      <c r="L12" s="6">
+      <c r="K12" s="5">
+        <v>2128459</v>
+      </c>
+      <c r="L12" s="5">
         <v>100000</v>
       </c>
     </row>
@@ -1265,13 +1226,13 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="F13" s="3">
         <v>53000</v>
@@ -1283,16 +1244,16 @@
         <v>16</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J13" s="3">
-        <v>3</v>
-      </c>
-      <c r="K13" s="6">
-        <v>10342993</v>
-      </c>
-      <c r="L13" s="6">
-        <v>600000</v>
+        <v>1</v>
+      </c>
+      <c r="K13" s="5">
+        <v>2128459</v>
+      </c>
+      <c r="L13" s="5">
+        <v>100000</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1303,13 +1264,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="F14" s="3">
         <v>53000</v>
@@ -1321,16 +1282,16 @@
         <v>16</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J14" s="3">
         <v>1</v>
       </c>
-      <c r="K14" s="6">
-        <v>2916600</v>
-      </c>
-      <c r="L14" s="6">
-        <v>100000</v>
+      <c r="K14" s="5">
+        <v>18771787</v>
+      </c>
+      <c r="L14" s="5">
+        <v>511794</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1341,13 +1302,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="F15" s="3">
         <v>53000</v>
@@ -1359,15 +1320,15 @@
         <v>16</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J15" s="3">
         <v>1</v>
       </c>
-      <c r="K15" s="6">
-        <v>2128459</v>
-      </c>
-      <c r="L15" s="6">
+      <c r="K15" s="5">
+        <v>2916600</v>
+      </c>
+      <c r="L15" s="5">
         <v>100000</v>
       </c>
     </row>
@@ -1379,34 +1340,34 @@
         <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="3">
+        <v>41500</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="3">
-        <v>53000</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="J16" s="3">
         <v>1</v>
       </c>
-      <c r="K16" s="6">
-        <v>18771787</v>
-      </c>
-      <c r="L16" s="6">
-        <v>511794</v>
+      <c r="K16" s="5">
+        <v>4457072</v>
+      </c>
+      <c r="L16" s="5">
+        <v>121393</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1417,92 +1378,54 @@
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="3">
+        <v>41500</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="3">
-        <v>53000</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="J17" s="3">
         <v>1</v>
       </c>
-      <c r="K17" s="6">
-        <v>2128459</v>
-      </c>
-      <c r="L17" s="6">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="3">
-        <v>41500</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J18" s="3">
-        <v>1</v>
-      </c>
-      <c r="K18" s="6">
-        <v>8162155</v>
-      </c>
-      <c r="L18" s="6">
-        <v>222441</v>
+      <c r="K17" s="5">
+        <v>9007610</v>
+      </c>
+      <c r="L17" s="5">
+        <v>245498</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F19" s="3">
-        <v>41500</v>
+        <v>105000</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>15</v>
@@ -1511,36 +1434,36 @@
         <v>16</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="J19" s="3">
-        <v>1</v>
-      </c>
-      <c r="K19" s="6">
-        <v>3165380</v>
-      </c>
-      <c r="L19" s="6">
-        <v>100000</v>
+        <v>3</v>
+      </c>
+      <c r="K19" s="5">
+        <v>72884193</v>
+      </c>
+      <c r="L19" s="5">
+        <v>3808922</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="3">
-        <v>41500</v>
+        <v>147000</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>15</v>
@@ -1549,36 +1472,36 @@
         <v>16</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="J20" s="3">
-        <v>1</v>
-      </c>
-      <c r="K20" s="6">
-        <v>4457072</v>
-      </c>
-      <c r="L20" s="6">
-        <v>121393</v>
+        <v>2</v>
+      </c>
+      <c r="K20" s="5">
+        <v>39113645</v>
+      </c>
+      <c r="L20" s="5">
+        <v>1607170</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="3">
-        <v>41500</v>
+        <v>105000</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>15</v>
@@ -1587,36 +1510,36 @@
         <v>16</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="J21" s="3">
-        <v>1</v>
-      </c>
-      <c r="K21" s="6">
-        <v>9007610</v>
-      </c>
-      <c r="L21" s="6">
-        <v>245498</v>
+        <v>2</v>
+      </c>
+      <c r="K21" s="5">
+        <v>28252672</v>
+      </c>
+      <c r="L21" s="5">
+        <v>1053426</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="3">
-        <v>197000</v>
+        <v>82500</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>15</v>
@@ -1625,33 +1548,33 @@
         <v>16</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="J22" s="3">
-        <v>1</v>
-      </c>
-      <c r="K22" s="6">
-        <v>12831598</v>
-      </c>
-      <c r="L22" s="6">
-        <v>356267</v>
+        <v>2</v>
+      </c>
+      <c r="K22" s="5">
+        <v>10812631</v>
+      </c>
+      <c r="L22" s="5">
+        <v>450838</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F23" s="3">
         <v>197000</v>
@@ -1663,36 +1586,36 @@
         <v>16</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="J23" s="3">
         <v>1</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23" s="5">
         <v>7895141</v>
       </c>
-      <c r="L23" s="6">
+      <c r="L23" s="5">
         <v>229781</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F24" s="3">
-        <v>147000</v>
+        <v>197000</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>15</v>
@@ -1701,30 +1624,30 @@
         <v>16</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="J24" s="3">
         <v>1</v>
       </c>
-      <c r="K24" s="6">
-        <v>9576370</v>
-      </c>
-      <c r="L24" s="6">
-        <v>265844</v>
+      <c r="K24" s="5">
+        <v>12831598</v>
+      </c>
+      <c r="L24" s="5">
+        <v>356267</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>14</v>
@@ -1739,30 +1662,30 @@
         <v>16</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="J25" s="3">
-        <v>2</v>
-      </c>
-      <c r="K25" s="6">
-        <v>39113645</v>
-      </c>
-      <c r="L25" s="6">
-        <v>1607170</v>
+        <v>1</v>
+      </c>
+      <c r="K25" s="5">
+        <v>9576370</v>
+      </c>
+      <c r="L25" s="5">
+        <v>265844</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>14</v>
@@ -1777,36 +1700,36 @@
         <v>16</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="J26" s="3">
-        <v>3</v>
-      </c>
-      <c r="K26" s="6">
-        <v>72884193</v>
-      </c>
-      <c r="L26" s="6">
-        <v>3808922</v>
+        <v>1</v>
+      </c>
+      <c r="K26" s="5">
+        <v>6841979</v>
+      </c>
+      <c r="L26" s="5">
+        <v>189888</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="F27" s="3">
-        <v>105000</v>
+        <v>66000</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>15</v>
@@ -1815,36 +1738,36 @@
         <v>16</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J27" s="3">
         <v>1</v>
       </c>
-      <c r="K27" s="6">
-        <v>6841979</v>
-      </c>
-      <c r="L27" s="6">
-        <v>189888</v>
+      <c r="K27" s="5">
+        <v>4700762</v>
+      </c>
+      <c r="L27" s="5">
+        <v>119358</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="3">
-        <v>105000</v>
+        <v>53000</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>15</v>
@@ -1853,247 +1776,108 @@
         <v>16</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J28" s="3">
-        <v>2</v>
-      </c>
-      <c r="K28" s="6">
-        <v>28252672</v>
-      </c>
-      <c r="L28" s="6">
-        <v>1053426</v>
+        <v>1</v>
+      </c>
+      <c r="K28" s="5">
+        <v>3456542</v>
+      </c>
+      <c r="L28" s="5">
+        <v>100000</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="3">
+        <v>41500</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1</v>
+      </c>
+      <c r="K29" s="5">
+        <v>940008</v>
+      </c>
+      <c r="L29" s="5">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="3">
-        <v>82500</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="J29" s="3">
-        <v>2</v>
-      </c>
-      <c r="K29" s="6">
-        <v>10812631</v>
-      </c>
-      <c r="L29" s="6">
-        <v>450838</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="E31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="3">
+        <v>41500</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="3">
-        <v>66000</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J30" s="3">
-        <v>1</v>
-      </c>
-      <c r="K30" s="6">
-        <v>4700762</v>
-      </c>
-      <c r="L30" s="6">
-        <v>119358</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
+      <c r="J31" s="3">
+        <v>1</v>
+      </c>
+      <c r="K31" s="5">
+        <v>2757873</v>
+      </c>
+      <c r="L31" s="5">
+        <v>100000</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>30</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="3">
-        <v>53000</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="J32" s="3">
-        <v>1</v>
-      </c>
       <c r="K32" s="6">
-        <v>3456542</v>
+        <f>SUM(K2:K31)</f>
+        <v>412510829</v>
       </c>
       <c r="L32" s="6">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>31</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F33" s="3">
-        <v>41500</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="J33" s="3">
-        <v>1</v>
-      </c>
-      <c r="K33" s="6">
-        <v>940008</v>
-      </c>
-      <c r="L33" s="6">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-    </row>
-    <row r="35" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>32</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="3">
-        <v>41500</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="J35" s="3">
-        <v>1</v>
-      </c>
-      <c r="K35" s="6">
-        <v>2757873</v>
-      </c>
-      <c r="L35" s="6">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K36" s="7">
-        <f>SUM(K2:K35)</f>
-        <v>454323448</v>
-      </c>
-      <c r="L36" s="7">
-        <f>SUM(L2:L35)</f>
-        <v>17213938</v>
+        <f>SUM(L2:L31)</f>
+        <v>15598469</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="B2:L17">
+    <sortCondition descending="1" ref="J2:J17"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>